<commit_message>
Cambio en los logs
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emxcdcd32sw1\Documents\UiPath\PDF_V2_PERFORMER\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emxxs232s\Documents\UiPath\PracticaOCR2Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8945D23-44B1-4B1D-9CDF-86A948C99C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C6997F-7E49-4F1A-9106-63D382614EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3705" yWindow="1770" windowWidth="15750" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Excel_Path</t>
+  </si>
+  <si>
+    <t>Dispacher_Performer</t>
   </si>
 </sst>
 </file>
@@ -218,10 +221,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -544,7 +547,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -604,7 +607,9 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>

</xml_diff>